<commit_message>
Fix date patterns for JDK6.
SimpleDateFormat in Java 6 does no support 'week year' - 'Y'.
It was replaced with 'y' in the Date.xlsx
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test/rules/functionality/Date.xlsx
+++ b/DEV/org.openl.test/test/rules/functionality/Date.xlsx
@@ -409,21 +409,12 @@
     <t>4/30/2015 13:30</t>
   </si>
   <si>
-    <t>dd.MM.YY</t>
-  </si>
-  <si>
     <t>30.04.15</t>
   </si>
   <si>
-    <t>dd$$$MM$$$YY$</t>
-  </si>
-  <si>
     <t>30$$$04$$$15$</t>
   </si>
   <si>
-    <t>dd$$$MM$$$YY</t>
-  </si>
-  <si>
     <t>30$$$04$$$15</t>
   </si>
   <si>
@@ -673,9 +664,6 @@
     <t>01/01/0001</t>
   </si>
   <si>
-    <t>MM/YY</t>
-  </si>
-  <si>
     <t>01/10</t>
   </si>
   <si>
@@ -821,6 +809,18 @@
   </si>
   <si>
     <t>31/12/2014</t>
+  </si>
+  <si>
+    <t>dd$$$MM$$$yy$</t>
+  </si>
+  <si>
+    <t>dd$$$MM$$$yy</t>
+  </si>
+  <si>
+    <t>dd.MM.yy</t>
+  </si>
+  <si>
+    <t>MM/yy</t>
   </si>
 </sst>
 </file>
@@ -1058,17 +1058,17 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1462,70 +1462,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="E2" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="F2" s="35"/>
-      <c r="H2" s="35" t="s">
+      <c r="C2" s="37"/>
+      <c r="E2" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="I2" s="35"/>
-      <c r="K2" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" s="35"/>
-      <c r="N2" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="O2" s="35"/>
+      <c r="F2" s="37"/>
+      <c r="H2" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="37"/>
+      <c r="K2" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="37"/>
+      <c r="N2" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" s="37"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="E3" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="F3" s="36"/>
-      <c r="H3" s="36" t="s">
+      <c r="C3" s="38"/>
+      <c r="E3" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="K3" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="L3" s="36"/>
-      <c r="N3" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="O3" s="36"/>
+      <c r="F3" s="38"/>
+      <c r="H3" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" s="38"/>
+      <c r="K3" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="L3" s="38"/>
+      <c r="N3" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" s="38"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="E5" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="F5" s="38"/>
-      <c r="H5" s="37" t="s">
+      <c r="C5" s="36"/>
+      <c r="E5" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="K5" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="L5" s="38"/>
-      <c r="N5" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="O5" s="38"/>
+      <c r="F5" s="36"/>
+      <c r="H5" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" s="36"/>
+      <c r="K5" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="L5" s="36"/>
+      <c r="N5" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" s="36"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -1567,25 +1567,25 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>1</v>
@@ -1611,13 +1611,13 @@
         <v>0</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L8" s="10">
         <v>0</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O8" s="10">
         <v>0</v>
@@ -1643,13 +1643,13 @@
         <v>0</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L9" s="10">
         <v>0</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O9" s="10">
         <v>0</v>
@@ -1675,13 +1675,13 @@
         <v>0</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L10" s="10">
         <v>0</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O10" s="10">
         <v>0</v>
@@ -1707,13 +1707,13 @@
         <v>1</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L11" s="10">
         <v>0</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O11" s="10">
         <v>0</v>
@@ -1739,13 +1739,13 @@
         <v>1</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L12" s="10">
         <v>0</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O12" s="10">
         <v>0</v>
@@ -1771,13 +1771,13 @@
         <v>1</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L13" s="10">
         <v>0</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O13" s="10">
         <v>0</v>
@@ -2748,7 +2748,7 @@
         <v>42197.499999999971</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E44" s="26">
         <v>42197.499999999971</v>
@@ -2780,7 +2780,7 @@
         <v>42197.500011574048</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E45" s="26">
         <v>42197.500011574048</v>
@@ -2812,7 +2812,7 @@
         <v>42197.541655092566</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E46" s="26">
         <v>42197.541655092566</v>
@@ -2844,7 +2844,7 @@
         <v>42197.541666666635</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E47" s="26">
         <v>42197.541666666635</v>
@@ -2876,7 +2876,7 @@
         <v>42197.541678240712</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E48" s="26">
         <v>42197.541678240712</v>
@@ -2908,7 +2908,7 @@
         <v>42197.58332175923</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E49" s="26">
         <v>42197.58332175923</v>
@@ -2940,7 +2940,7 @@
         <v>42197.583333333299</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E50" s="26">
         <v>42197.583333333299</v>
@@ -2972,7 +2972,7 @@
         <v>42197.583344907376</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E51" s="26">
         <v>42197.583344907376</v>
@@ -3004,7 +3004,7 @@
         <v>42197.624988425894</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E52" s="26">
         <v>42197.624988425894</v>
@@ -3036,7 +3036,7 @@
         <v>42197.624999999964</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E53" s="26">
         <v>42197.624999999964</v>
@@ -3068,7 +3068,7 @@
         <v>42197.62501157404</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E54" s="26">
         <v>42197.62501157404</v>
@@ -3100,7 +3100,7 @@
         <v>42197.666655092558</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E55" s="26">
         <v>42197.666655092558</v>
@@ -3132,7 +3132,7 @@
         <v>42197.666666666628</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E56" s="26">
         <v>42197.666666666628</v>
@@ -3164,7 +3164,7 @@
         <v>42197.666678240705</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E57" s="26">
         <v>42197.666678240705</v>
@@ -3196,7 +3196,7 @@
         <v>42197.708321759223</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E58" s="26">
         <v>42197.708321759223</v>
@@ -3228,7 +3228,7 @@
         <v>42197.708333333292</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E59" s="26">
         <v>42197.708333333292</v>
@@ -3260,7 +3260,7 @@
         <v>42197.708344907369</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E60" s="26">
         <v>42197.708344907369</v>
@@ -3292,7 +3292,7 @@
         <v>42197.749988425887</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E61" s="26">
         <v>42197.749988425887</v>
@@ -3324,7 +3324,7 @@
         <v>42197.749999999956</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E62" s="26">
         <v>42197.749999999956</v>
@@ -3356,7 +3356,7 @@
         <v>42197.750011574033</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E63" s="26">
         <v>42197.750011574033</v>
@@ -3388,7 +3388,7 @@
         <v>42197.791655092551</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E64" s="26">
         <v>42197.791655092551</v>
@@ -3420,7 +3420,7 @@
         <v>42197.791666666621</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E65" s="26">
         <v>42197.791666666621</v>
@@ -3452,7 +3452,7 @@
         <v>42197.791678240697</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E66" s="26">
         <v>42197.791678240697</v>
@@ -3484,7 +3484,7 @@
         <v>42197.833321759215</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E67" s="26">
         <v>42197.833321759215</v>
@@ -3516,7 +3516,7 @@
         <v>42197.833333333285</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E68" s="26">
         <v>42197.833333333285</v>
@@ -3548,7 +3548,7 @@
         <v>42197.833344907362</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E69" s="26">
         <v>42197.833344907362</v>
@@ -3580,7 +3580,7 @@
         <v>42197.87498842588</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E70" s="26">
         <v>42197.87498842588</v>
@@ -3612,7 +3612,7 @@
         <v>42197.874999999949</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E71" s="26">
         <v>42197.874999999949</v>
@@ -3644,7 +3644,7 @@
         <v>42197.875011574026</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E72" s="26">
         <v>42197.875011574026</v>
@@ -3676,7 +3676,7 @@
         <v>42197.916655092544</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E73" s="26">
         <v>42197.916655092544</v>
@@ -3708,7 +3708,7 @@
         <v>42197.916666666613</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E74" s="26">
         <v>42197.916666666613</v>
@@ -3740,7 +3740,7 @@
         <v>42197.91667824069</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E75" s="26">
         <v>42197.91667824069</v>
@@ -3772,7 +3772,7 @@
         <v>42197.958321759208</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E76" s="26">
         <v>42197.958321759208</v>
@@ -3804,7 +3804,7 @@
         <v>42197.958333333278</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E77" s="26">
         <v>42197.958333333278</v>
@@ -3836,7 +3836,7 @@
         <v>42197.958344907354</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E78" s="26">
         <v>42197.958344907354</v>
@@ -3868,7 +3868,7 @@
         <v>42197.999988425872</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E79" s="26">
         <v>42197.999988425872</v>
@@ -3897,7 +3897,7 @@
     </row>
     <row r="83" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K83" s="31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L83" s="30">
         <v>42</v>
@@ -3905,7 +3905,7 @@
     </row>
     <row r="84" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K84" s="31" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L84" s="30">
         <v>30</v>
@@ -3913,7 +3913,7 @@
     </row>
     <row r="85" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K85" s="25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L85" s="6">
         <v>0</v>
@@ -3921,12 +3921,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="K5:L5"/>
@@ -3936,6 +3930,12 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3962,46 +3962,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="E2" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="F2" s="35"/>
-      <c r="H2" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="35"/>
+      <c r="B2" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="E2" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="H2" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" s="37"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="E3" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="F3" s="36"/>
-      <c r="H3" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="36"/>
+      <c r="B3" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="E3" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="38"/>
+      <c r="H3" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="38"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="E5" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="F5" s="38"/>
-      <c r="H5" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" s="38"/>
+      <c r="B5" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="E5" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="H5" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="36"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -4025,13 +4025,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>1</v>
@@ -4046,19 +4046,19 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F8" s="10">
         <v>4</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I8" s="10">
         <v>14</v>
@@ -4067,19 +4067,19 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F9" s="10">
         <v>11</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I9" s="10">
         <v>30</v>
@@ -4088,19 +4088,19 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C10" s="11">
         <v>1789</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F10" s="10">
         <v>4</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I10" s="10">
         <v>14</v>
@@ -4109,19 +4109,19 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C11" s="11">
         <v>1</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F11" s="10">
         <v>0</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I11" s="10">
         <v>1</v>
@@ -4129,19 +4129,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F12" s="10">
         <v>11</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I12" s="10">
         <v>30</v>
@@ -4149,19 +4149,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13" s="11">
         <v>10</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I13" s="6">
         <v>1</v>
@@ -4209,19 +4209,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C16" s="11">
         <v>1899</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F16" s="10">
         <v>11</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I16" s="6">
         <v>30</v>
@@ -4229,19 +4229,19 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C17" s="11">
         <v>1894</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F17" s="10">
         <v>4</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I17" s="6">
         <v>25</v>
@@ -4269,19 +4269,19 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C19" s="13">
         <v>3892</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F19" s="10">
         <v>4</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I19" s="6">
         <v>14</v>
@@ -4330,70 +4330,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="E2" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="35"/>
-      <c r="H2" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="I2" s="35"/>
-      <c r="K2" s="35" t="s">
+      <c r="B2" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="E2" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="H2" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="37"/>
+      <c r="K2" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="37"/>
+      <c r="N2" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="35"/>
-      <c r="N2" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="35"/>
+      <c r="O2" s="37"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="E3" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="36"/>
-      <c r="H3" s="36" t="s">
+      <c r="B3" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="E3" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="38"/>
+      <c r="H3" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="38"/>
+      <c r="K3" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="L3" s="38"/>
+      <c r="N3" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" s="38"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B5" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="K3" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="L3" s="36"/>
-      <c r="N3" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="O3" s="36"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="E5" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="38"/>
-      <c r="H5" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="38"/>
-      <c r="K5" s="37" t="s">
+      <c r="C5" s="36"/>
+      <c r="E5" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="36"/>
+      <c r="H5" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="36"/>
+      <c r="K5" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="L5" s="36"/>
+      <c r="N5" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="N5" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="O5" s="38"/>
+      <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -4435,7 +4435,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>1</v>
@@ -4447,13 +4447,13 @@
         <v>1</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>1</v>
@@ -4462,13 +4462,13 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" s="10">
         <v>134</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -4480,13 +4480,13 @@
         <v>5</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L8" s="10">
         <v>20</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O8" s="10">
         <v>3</v>
@@ -4495,13 +4495,13 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C9" s="10">
         <v>364</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F9" s="10">
         <v>3</v>
@@ -4513,13 +4513,13 @@
         <v>5</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L9" s="10">
         <v>1</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="O9" s="10">
         <v>5</v>
@@ -4528,13 +4528,13 @@
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C10" s="10">
         <v>134</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
@@ -4546,13 +4546,13 @@
         <v>1</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L10" s="10">
         <v>20</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O10" s="10">
         <v>3</v>
@@ -4561,31 +4561,31 @@
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C11" s="10">
         <v>1</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F11" s="17">
         <v>0</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I11" s="10">
         <v>7</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L11" s="10">
         <v>1</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O11" s="10">
         <v>1</v>
@@ -4594,13 +4594,13 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12" s="10">
         <v>364</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F12" s="10">
         <v>3</v>
@@ -4612,13 +4612,13 @@
         <v>4</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L12" s="10">
         <v>1</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O12" s="10">
         <v>5</v>
@@ -4627,13 +4627,13 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13" s="10">
         <v>1</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F13" s="17">
         <v>0</v>
@@ -4645,13 +4645,13 @@
         <v>5</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L13" s="10">
         <v>1</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O13" s="10">
         <v>1</v>
@@ -4672,7 +4672,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I14" s="20">
         <v>5</v>
@@ -4705,7 +4705,7 @@
         <v>3</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I15" s="20">
         <v>4</v>
@@ -4726,13 +4726,13 @@
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C16" s="16">
         <v>364</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F16" s="10">
         <v>3</v>
@@ -4744,13 +4744,13 @@
         <v>2</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L16" s="10">
         <v>52</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="O16" s="10">
         <v>5</v>
@@ -4759,13 +4759,13 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C17" s="16">
         <v>145</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F17" s="10">
         <v>1</v>
@@ -4777,13 +4777,13 @@
         <v>1</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="L17" s="10">
         <v>21</v>
       </c>
       <c r="N17" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="O17" s="10">
         <v>4</v>
@@ -4804,7 +4804,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I18" s="20">
         <v>7</v>
@@ -4825,31 +4825,31 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C19" s="16">
         <v>135</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F19" s="10">
         <v>1</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I19" s="20">
         <v>6</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L19" s="10">
         <v>20</v>
       </c>
       <c r="N19" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O19" s="10">
         <v>2</v>
@@ -4865,7 +4865,7 @@
       <c r="B21" s="32"/>
       <c r="C21" s="33"/>
       <c r="H21" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I21" s="10">
         <v>2</v>
@@ -4874,7 +4874,7 @@
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="H22" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I22" s="20">
         <v>6</v>
@@ -4941,22 +4941,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" s="35"/>
+      <c r="B2" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="36"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -5008,7 +5008,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C12" s="9">
         <v>120</v>
@@ -5040,29 +5040,29 @@
     </row>
     <row r="16" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C16" s="6">
         <v>46708</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="35"/>
+      <c r="B20" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="37"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="36"/>
+      <c r="C21" s="38"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="38"/>
+      <c r="C23" s="36"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
@@ -5082,7 +5082,7 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C26" s="16">
         <v>8061</v>
@@ -5090,7 +5090,7 @@
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C27" s="7">
         <v>8063</v>
@@ -5098,7 +5098,7 @@
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C28" s="10">
         <v>7157</v>
@@ -5106,7 +5106,7 @@
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C29" s="6">
         <v>4</v>
@@ -5114,7 +5114,7 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C30" s="6">
         <v>8063</v>
@@ -5122,7 +5122,7 @@
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C31" s="6">
         <v>40</v>
@@ -5146,7 +5146,7 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C34" s="6">
         <v>7599</v>
@@ -5154,7 +5154,7 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C35" s="6">
         <v>7577</v>
@@ -5170,7 +5170,7 @@
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C37" s="6">
         <v>15569</v>
@@ -5208,32 +5208,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
+      <c r="B3" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
-        <v>65</v>
+      <c r="B5" s="35" t="s">
+        <v>62</v>
       </c>
       <c r="C5" s="39"/>
-      <c r="D5" s="38"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>0</v>
@@ -5244,7 +5244,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>1</v>
@@ -5255,7 +5255,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
@@ -5290,10 +5290,10 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D12" s="10">
         <v>0</v>
@@ -5301,10 +5301,10 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D13" s="10">
         <v>365</v>
@@ -5323,10 +5323,10 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D15" s="10">
         <v>364</v>
@@ -5334,10 +5334,10 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D16" s="21">
         <v>78891</v>
@@ -5353,7 +5353,7 @@
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="18"/>
       <c r="C18" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D18" s="20">
         <v>0</v>
@@ -5361,7 +5361,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="20">
@@ -5370,10 +5370,10 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D20" s="10">
         <v>-32872</v>
@@ -5381,10 +5381,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D21" s="10">
         <v>32872</v>
@@ -5392,7 +5392,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C22" s="24">
         <v>1</v>
@@ -5403,7 +5403,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C23" s="23">
         <v>1</v>
@@ -5414,7 +5414,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C24" s="23">
         <v>2</v>
@@ -5435,32 +5435,32 @@
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
+      <c r="B29" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
+      <c r="B30" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="37" t="s">
-        <v>98</v>
+      <c r="B32" s="35" t="s">
+        <v>95</v>
       </c>
       <c r="C32" s="39"/>
-      <c r="D32" s="38"/>
+      <c r="D32" s="36"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>0</v>
@@ -5468,10 +5468,10 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>1</v>
@@ -5479,10 +5479,10 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D35" s="10">
         <v>0</v>
@@ -5490,10 +5490,10 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D36" s="10">
         <v>52</v>
@@ -5512,10 +5512,10 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D38" s="10">
         <v>52</v>
@@ -5523,10 +5523,10 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D39" s="21">
         <v>11270</v>
@@ -5542,7 +5542,7 @@
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="18"/>
       <c r="C41" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D41" s="20">
         <v>0</v>
@@ -5550,7 +5550,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="20">
@@ -5559,10 +5559,10 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D43" s="10">
         <v>-4696</v>
@@ -5570,10 +5570,10 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D44" s="10">
         <v>4696</v>
@@ -5581,7 +5581,7 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C45" s="24">
         <v>1</v>
@@ -5592,7 +5592,7 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C46" s="23">
         <v>1</v>
@@ -5603,7 +5603,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C47" s="23">
         <v>2</v>
@@ -5624,32 +5624,32 @@
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
+      <c r="B52" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
+      <c r="B53" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="37" t="s">
-        <v>112</v>
+      <c r="B55" s="35" t="s">
+        <v>109</v>
       </c>
       <c r="C55" s="39"/>
-      <c r="D55" s="38"/>
+      <c r="D55" s="36"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>0</v>
@@ -5657,10 +5657,10 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>1</v>
@@ -5668,10 +5668,10 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D58" s="10">
         <v>0</v>
@@ -5679,10 +5679,10 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D59" s="10">
         <v>12</v>
@@ -5701,10 +5701,10 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D61" s="10">
         <v>12</v>
@@ -5712,10 +5712,10 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D62" s="21">
         <v>2591</v>
@@ -5731,7 +5731,7 @@
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" s="18"/>
       <c r="C64" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D64" s="20">
         <v>0</v>
@@ -5739,7 +5739,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="20">
@@ -5748,10 +5748,10 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D66" s="20">
         <v>-1080</v>
@@ -5759,10 +5759,10 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D67" s="20">
         <v>1080</v>
@@ -5770,7 +5770,7 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B68" s="22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C68" s="24">
         <v>1</v>
@@ -5781,7 +5781,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" s="22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C69" s="23">
         <v>1</v>
@@ -5792,7 +5792,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70" s="22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C70" s="23">
         <v>2</v>
@@ -5813,32 +5813,32 @@
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B75" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
+      <c r="B75" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C75" s="37"/>
+      <c r="D75" s="37"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B76" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="C76" s="36"/>
-      <c r="D76" s="36"/>
+      <c r="B76" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C76" s="38"/>
+      <c r="D76" s="38"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B78" s="37" t="s">
-        <v>82</v>
+      <c r="B78" s="35" t="s">
+        <v>79</v>
       </c>
       <c r="C78" s="39"/>
-      <c r="D78" s="38"/>
+      <c r="D78" s="36"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>0</v>
@@ -5846,10 +5846,10 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B80" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>1</v>
@@ -5857,10 +5857,10 @@
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D81" s="10">
         <v>0</v>
@@ -5868,10 +5868,10 @@
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D82" s="10">
         <v>1</v>
@@ -5890,10 +5890,10 @@
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B84" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D84" s="10">
         <v>0</v>
@@ -5901,10 +5901,10 @@
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D85" s="10">
         <v>215</v>
@@ -5920,7 +5920,7 @@
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B87" s="18"/>
       <c r="C87" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D87" s="20">
         <v>0</v>
@@ -5928,7 +5928,7 @@
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B88" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C88" s="19"/>
       <c r="D88" s="20">
@@ -5937,10 +5937,10 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D89" s="10">
         <v>-90</v>
@@ -5948,10 +5948,10 @@
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B90" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D90" s="10">
         <v>90</v>
@@ -5970,6 +5970,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B78:D78"/>
     <mergeCell ref="B32:D32"/>
@@ -5977,11 +5982,6 @@
     <mergeCell ref="B53:D53"/>
     <mergeCell ref="B55:D55"/>
     <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6004,26 +6004,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="35"/>
+      <c r="B2" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="36"/>
+      <c r="B3" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="38"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="38"/>
+      <c r="B5" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -6031,7 +6031,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
@@ -6043,7 +6043,7 @@
         <v>8060</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -6052,7 +6052,7 @@
         <v>8061</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -6061,7 +6061,7 @@
         <v>8062</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -6070,7 +6070,7 @@
         <v>8063</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -6078,7 +6078,7 @@
         <v>8064</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -6087,7 +6087,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -6096,7 +6096,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -6105,7 +6105,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -6114,7 +6114,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -6122,30 +6122,30 @@
         <v>4</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" s="35"/>
+      <c r="B22" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="37"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="C23" s="36"/>
+      <c r="B23" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="38"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="C25" s="38"/>
+      <c r="B25" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="36"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -6153,7 +6153,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>1</v>
@@ -6164,7 +6164,7 @@
         <v>8060</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -6172,7 +6172,7 @@
         <v>8061</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -6180,7 +6180,7 @@
         <v>8062</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -6188,7 +6188,7 @@
         <v>8063</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -6196,7 +6196,7 @@
         <v>8064</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
@@ -6204,7 +6204,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.2">
@@ -6212,7 +6212,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.2">
@@ -6220,7 +6220,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
@@ -6228,7 +6228,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.2">
@@ -6236,7 +6236,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -6270,22 +6270,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="35"/>
+      <c r="B2" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="36"/>
+      <c r="B3" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="38"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="38"/>
+      <c r="B5" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -6297,7 +6297,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>1</v>
@@ -6306,7 +6306,7 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" s="10">
         <v>31</v>
@@ -6315,7 +6315,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C9" s="10">
         <v>31</v>
@@ -6324,7 +6324,7 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C10" s="10">
         <v>31</v>
@@ -6333,7 +6333,7 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C11" s="10">
         <v>31</v>
@@ -6342,7 +6342,7 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12" s="10">
         <v>31</v>
@@ -6351,7 +6351,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13" s="10">
         <v>31</v>
@@ -6378,7 +6378,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C16" s="10">
         <v>31</v>
@@ -6387,7 +6387,7 @@
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C17" s="10">
         <v>31</v>
@@ -6405,7 +6405,7 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C19" s="10">
         <v>31</v>
@@ -6413,7 +6413,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C20" s="10">
         <v>30</v>
@@ -6429,7 +6429,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C22" s="10">
         <v>30</v>
@@ -6437,7 +6437,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C23" s="10">
         <v>28</v>
@@ -6445,7 +6445,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" s="11" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C24" s="10">
         <v>30</v>
@@ -6453,7 +6453,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C25" s="10">
         <v>28</v>
@@ -6501,7 +6501,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B31" s="11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C31" s="10">
         <v>30</v>
@@ -6522,8 +6522,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6534,22 +6534,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="35"/>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="36"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
@@ -6633,10 +6633,10 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -6665,31 +6665,31 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>20</v>
@@ -6700,7 +6700,7 @@
         <v>0.61284722222222221</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
@@ -6708,7 +6708,7 @@
         <v>0.61249999999999993</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
@@ -6716,7 +6716,7 @@
         <v>0.83332175925925922</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -6724,29 +6724,29 @@
         <v>0.1125</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="39"/>
-      <c r="D34" s="38"/>
+      <c r="D34" s="36"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
@@ -6871,7 +6871,7 @@
         <v>34</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
@@ -6882,7 +6882,7 @@
         <v>34</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
@@ -6919,10 +6919,10 @@
         <v>47</v>
       </c>
       <c r="C51" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D51" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
@@ -6933,7 +6933,7 @@
         <v>34</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
@@ -6941,10 +6941,10 @@
         <v>26</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
@@ -6955,18 +6955,18 @@
         <v>34</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>136</v>
+        <v>185</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
@@ -6985,10 +6985,10 @@
         <v>25</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
@@ -7004,46 +7004,46 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
@@ -7051,10 +7051,10 @@
         <v>0.61284722222222221</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
@@ -7062,10 +7062,10 @@
         <v>0.61249999999999993</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
@@ -7073,10 +7073,10 @@
         <v>0.83332175925925922</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
@@ -7087,7 +7087,7 @@
         <v>34</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
@@ -7095,10 +7095,10 @@
         <v>47</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>50</v>
+        <v>182</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
@@ -7106,10 +7106,10 @@
         <v>47</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>52</v>
+        <v>183</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>